<commit_message>
Able to play full single player game
</commit_message>
<xml_diff>
--- a/celljointAngles.xlsx
+++ b/celljointAngles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DJDuong\Documents\Uni\41013 Robotics\Assignments\2\snl_gui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A7C207-9DE9-41A3-A0E8-F8C9D90C925E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A485B4-D604-4AE0-AF89-8948F5AEA9C7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="6250" xr2:uid="{3A7B7327-2FFC-46CF-943D-791C85F2C4B2}"/>
   </bookViews>
@@ -374,699 +374,699 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:G30"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1">
-        <v>0.61666027673002777</v>
+        <v>0.50774764079014723</v>
       </c>
       <c r="B1">
-        <v>1.5186409800067848</v>
+        <v>1.5447186534008406</v>
       </c>
       <c r="C1">
-        <v>0.44485442848683593</v>
+        <v>0.77312631709436319</v>
       </c>
       <c r="D1">
-        <v>0.89891274170098567</v>
+        <v>0.91732051115561342</v>
       </c>
       <c r="E1">
-        <v>1.3514370741272499</v>
+        <v>1.0983302441261191</v>
       </c>
       <c r="F1">
-        <v>-1.0461748973380072</v>
+        <v>-1.1029321864897761</v>
       </c>
       <c r="G1">
-        <v>1.9098060809176232</v>
+        <v>1.753340040553288</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>0.38963112012295287</v>
+        <v>0.3865631585471816</v>
       </c>
       <c r="B2">
-        <v>1.4925633066127288</v>
+        <v>1.5309128263098699</v>
       </c>
       <c r="C2">
-        <v>0.34514567727426926</v>
+        <v>0.74398068212453594</v>
       </c>
       <c r="D2">
-        <v>1.1504855909142309</v>
+        <v>1.2072428800659996</v>
       </c>
       <c r="E2">
-        <v>1.3545050357030211</v>
+        <v>1.4404079598246171</v>
       </c>
       <c r="F2">
-        <v>-1.1412817061869169</v>
+        <v>-1.1919030721871431</v>
       </c>
       <c r="G2">
-        <v>2.1061556217669852</v>
+        <v>2.1981944690401236</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>0.19174759848570513</v>
+        <v>0.18867963690993386</v>
       </c>
       <c r="B3">
-        <v>1.4388739790367313</v>
+        <v>1.4173982480063325</v>
       </c>
       <c r="C3">
-        <v>7.6699039394282062E-2</v>
+        <v>0.30372819600135698</v>
       </c>
       <c r="D3">
-        <v>1.3606409588545638</v>
+        <v>1.3453011509757073</v>
       </c>
       <c r="E3">
-        <v>1.1228739367322893</v>
+        <v>0.90965060721618518</v>
       </c>
       <c r="F3">
-        <v>-1.1919030721871431</v>
+        <v>-1.1550875332778878</v>
       </c>
       <c r="G3">
-        <v>2.1736507764339534</v>
+        <v>2.1245633912216131</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>-6.9029135454853854E-2</v>
+        <v>-5.9825250727540004E-2</v>
       </c>
       <c r="B4">
-        <v>1.3284273623089653</v>
+        <v>1.3882526130365052</v>
       </c>
       <c r="C4">
-        <v>-0.23930100291016002</v>
+        <v>-0.19481556006147643</v>
       </c>
       <c r="D4">
-        <v>1.6735730395832344</v>
+        <v>1.4266021327336462</v>
       </c>
       <c r="E4">
-        <v>0.57064085309345847</v>
+        <v>4.7553404424454875E-2</v>
       </c>
       <c r="F4">
-        <v>-1.4496118445519308</v>
+        <v>-1.3284273623089653</v>
       </c>
       <c r="G4">
-        <v>2.0417284286757882</v>
+        <v>1.8024274257656283</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>-7.9767000970053348E-2</v>
+        <v>-0.20095148321301901</v>
       </c>
       <c r="B5">
-        <v>1.4634176716429017</v>
+        <v>1.4910293258248433</v>
       </c>
       <c r="C5">
-        <v>-0.75471854763973545</v>
+        <v>-0.5905826033359719</v>
       </c>
       <c r="D5">
-        <v>1.5186409800067848</v>
+        <v>1.2624661884298827</v>
       </c>
       <c r="E5">
-        <v>0.28225246497095796</v>
+        <v>-0.3175340230923277</v>
       </c>
       <c r="F5">
-        <v>-1.4710875755823298</v>
+        <v>-1.3253594007331939</v>
       </c>
       <c r="G5">
-        <v>2.2288740847978366</v>
+        <v>1.8315730607354554</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>-0.65807775800294011</v>
+        <v>-0.69335931612430979</v>
       </c>
       <c r="B6">
-        <v>1.5263108839462129</v>
+        <v>1.6106798272799232</v>
       </c>
       <c r="C6">
-        <v>-1.3759807667334201</v>
+        <v>-0.61666027673002777</v>
       </c>
       <c r="D6">
-        <v>0.97867974267103908</v>
+        <v>0.72250495109413704</v>
       </c>
       <c r="E6">
-        <v>-1.3284273623089653</v>
+        <v>-0.86056322200384472</v>
       </c>
       <c r="F6">
-        <v>-1.2747380347329678</v>
+        <v>-1.021631204731837</v>
       </c>
       <c r="G6">
-        <v>1.3284273623089653</v>
+        <v>1.4342720366730746</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>-0.76852437473070623</v>
+        <v>-0.75778650921550672</v>
       </c>
       <c r="B7">
-        <v>1.3913205746122765</v>
+        <v>1.3836506706728484</v>
       </c>
       <c r="C7">
-        <v>-1.248660361338912</v>
+        <v>-0.53996123733574564</v>
       </c>
       <c r="D7">
-        <v>1.0293011086712651</v>
+        <v>0.89891274170098567</v>
       </c>
       <c r="E7">
-        <v>-1.517106999218899</v>
+        <v>-1.0983302441261191</v>
       </c>
       <c r="F7">
-        <v>-1.1382137446111458</v>
+        <v>-0.92345643430715596</v>
       </c>
       <c r="G7">
-        <v>1.069184609156292</v>
+        <v>1.227184630308513</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>-0.16106798272799233</v>
+        <v>-0.56297094915403034</v>
       </c>
       <c r="B8">
-        <v>1.2793399770966247</v>
+        <v>1.3222914391574228</v>
       </c>
       <c r="C8">
-        <v>-0.42644665903220824</v>
+        <v>-0.52768939103266055</v>
       </c>
       <c r="D8">
-        <v>1.8407769454627694</v>
+        <v>1.1658253987930873</v>
       </c>
       <c r="E8">
-        <v>0.88357293382212931</v>
+        <v>-1.1382137446111458</v>
       </c>
       <c r="F8">
-        <v>-1.6444274046134073</v>
+        <v>-1.0446409165501216</v>
       </c>
       <c r="G8">
-        <v>2.4559032414049113</v>
+        <v>1.1213399559444037</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>-9.0504866485252827E-2</v>
+        <v>-0.26844663787998718</v>
       </c>
       <c r="B9">
-        <v>1.1060001480655473</v>
+        <v>1.1428156869748027</v>
       </c>
       <c r="C9">
-        <v>-0.13499030933393641</v>
+        <v>-0.35281558121369749</v>
       </c>
       <c r="D9">
-        <v>1.9251458887964796</v>
+        <v>1.5539225381281545</v>
       </c>
       <c r="E9">
-        <v>0.85902924121595903</v>
+        <v>-0.80227195206419033</v>
       </c>
       <c r="F9">
-        <v>-1.4465438829761597</v>
+        <v>-1.1826991874598294</v>
       </c>
       <c r="G9">
-        <v>2.1981944690401236</v>
+        <v>1.0400389741864646</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>-0.12732040539450823</v>
+        <v>-0.22089323345553233</v>
       </c>
       <c r="B10">
+        <v>1.000155473701438</v>
+      </c>
+      <c r="C10">
+        <v>0.19634954084936207</v>
+      </c>
+      <c r="D10">
+        <v>1.7472041174017452</v>
+      </c>
+      <c r="E10">
+        <v>-0.17794177139473438</v>
+      </c>
+      <c r="F10">
+        <v>-1.1919030721871431</v>
+      </c>
+      <c r="G10">
         <v>1.1259418983080607</v>
-      </c>
-      <c r="C10">
-        <v>-0.39730102406238105</v>
-      </c>
-      <c r="D10">
-        <v>1.906738119341852</v>
-      </c>
-      <c r="E10">
-        <v>-0.6135923151542565</v>
-      </c>
-      <c r="F10">
-        <v>-1.5401167110371838</v>
-      </c>
-      <c r="G10">
-        <v>0.97407780030738211</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>-0.19481556006147643</v>
+        <v>0.14266021327336462</v>
       </c>
       <c r="B11">
-        <v>1.1826991874598294</v>
+        <v>1.2716700731571966</v>
       </c>
       <c r="C11">
-        <v>4.141748127291231E-2</v>
+        <v>0.6135923151542565</v>
       </c>
       <c r="D11">
-        <v>1.8883303498872244</v>
+        <v>1.3529710549151355</v>
       </c>
       <c r="E11">
-        <v>-0.47860200582032003</v>
+        <v>0.82221370230670365</v>
       </c>
       <c r="F11">
-        <v>-1.5600584612796971</v>
+        <v>-1.1919030721871431</v>
       </c>
       <c r="G11">
-        <v>0.6688156235181395</v>
+        <v>1.6122138080678088</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>-0.13192234775816514</v>
+        <v>0.4878058905476339</v>
       </c>
       <c r="B12">
-        <v>1.4695535947944443</v>
+        <v>1.3345632854605078</v>
       </c>
       <c r="C12">
-        <v>0.57524279545711543</v>
+        <v>0.68415543139699597</v>
       </c>
       <c r="D12">
-        <v>1.6566992509164924</v>
+        <v>0.94800012691332625</v>
       </c>
       <c r="E12">
-        <v>-0.32213596545598466</v>
+        <v>1.0523108204895499</v>
       </c>
       <c r="F12">
-        <v>-1.6014759425526093</v>
+        <v>-0.89737876091310009</v>
       </c>
       <c r="G12">
-        <v>0.29605829206192874</v>
+        <v>1.6398254622497503</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>0.12885438618239387</v>
+        <v>0.56297094915403034</v>
       </c>
       <c r="B13">
-        <v>1.3667768820061064</v>
+        <v>1.0906603401866908</v>
       </c>
       <c r="C13">
-        <v>-7.5165058606396412E-2</v>
+        <v>0.51388356394168977</v>
       </c>
       <c r="D13">
-        <v>1.5968740001889525</v>
+        <v>1.1244079175201749</v>
       </c>
       <c r="E13">
-        <v>-1.5508545765523831</v>
+        <v>1.1290098598838318</v>
       </c>
       <c r="F13">
-        <v>-1.8438449070385408</v>
+        <v>-0.67034960430602519</v>
       </c>
       <c r="G13">
-        <v>-0.31446606151655643</v>
+        <v>1.7502720789775166</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>0.53075735260843182</v>
+        <v>0.33287383097118411</v>
       </c>
       <c r="B14">
-        <v>1.2501943421267976</v>
+        <v>0.95413605006486879</v>
       </c>
       <c r="C14">
-        <v>0.43104860139586515</v>
+        <v>0.38196121618352463</v>
       </c>
       <c r="D14">
-        <v>1.5539225381281545</v>
+        <v>1.4986992297642714</v>
       </c>
       <c r="E14">
-        <v>1.8837284075235674</v>
+        <v>0.95413605006486879</v>
       </c>
       <c r="F14">
-        <v>-0.87130108751904423</v>
+        <v>-0.81607777915516111</v>
       </c>
       <c r="G14">
-        <v>2.6384469551633027</v>
+        <v>1.9665633700693921</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>0.24850488763747386</v>
+        <v>0.11658253987930872</v>
       </c>
       <c r="B15">
-        <v>0.69335931612430979</v>
+        <v>0.8958447801252144</v>
       </c>
       <c r="C15">
-        <v>-0.14266021327336462</v>
+        <v>0.17333982903107745</v>
       </c>
       <c r="D15">
-        <v>2.0156507552817327</v>
+        <v>1.7073206169167185</v>
       </c>
       <c r="E15">
-        <v>0.82528166388247493</v>
+        <v>0.59671852648751444</v>
       </c>
       <c r="F15">
-        <v>-0.87743701067058677</v>
+        <v>-1.0630486860047492</v>
       </c>
       <c r="G15">
-        <v>2.138369218312584</v>
+        <v>1.8913983114629955</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>-3.2213596545598466E-2</v>
+        <v>-0.31293208072867079</v>
       </c>
       <c r="B16">
-        <v>0.78079622103379132</v>
+        <v>0.91578653036772772</v>
       </c>
       <c r="C16">
-        <v>-0.15033011721279282</v>
+        <v>-0.33133985018329848</v>
       </c>
       <c r="D16">
-        <v>2.0540002749788737</v>
+        <v>1.5968740001889525</v>
       </c>
       <c r="E16">
-        <v>0.73477679739722213</v>
+        <v>-0.80994185600361857</v>
       </c>
       <c r="F16">
-        <v>-1.1949710337629145</v>
+        <v>-0.98941760818623858</v>
       </c>
       <c r="G16">
-        <v>2.0678061020698442</v>
+        <v>1.1121360712170898</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>-3.8349519697141031E-2</v>
+        <v>-0.60285444963905699</v>
       </c>
       <c r="B17">
-        <v>1.0737865515199487</v>
+        <v>0.95720401164064006</v>
       </c>
       <c r="C17">
-        <v>-0.56910687230557289</v>
+        <v>-0.25770877236478773</v>
       </c>
       <c r="D17">
-        <v>2.0064468705544187</v>
+        <v>1.4312040750973032</v>
       </c>
       <c r="E17">
-        <v>0.8390874909734457</v>
+        <v>-0.94339818454966928</v>
       </c>
       <c r="F17">
-        <v>-1.5600584612796971</v>
+        <v>-0.77312631709436319</v>
       </c>
       <c r="G17">
-        <v>2.5648158773447922</v>
+        <v>0.99555353133778113</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>-0.13499030933393641</v>
+        <v>-0.78079622103379132</v>
       </c>
       <c r="B18">
-        <v>1.2394564766115981</v>
+        <v>1.1213399559444037</v>
       </c>
       <c r="C18">
-        <v>-0.88357293382212931</v>
+        <v>-0.46786414030512058</v>
       </c>
       <c r="D18">
-        <v>1.8545827725537403</v>
+        <v>1.021631204731837</v>
       </c>
       <c r="E18">
-        <v>0.71330106636682311</v>
+        <v>-1.1136700520049756</v>
       </c>
       <c r="F18">
-        <v>-1.6566992509164924</v>
+        <v>-0.6688156235181395</v>
       </c>
       <c r="G18">
-        <v>2.7258838600727842</v>
+        <v>1.2210487071569704</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>-0.57370881466922985</v>
+        <v>-0.68722339297276724</v>
       </c>
       <c r="B19">
-        <v>1.064582666792635</v>
+        <v>0.94800012691332625</v>
       </c>
       <c r="C19">
-        <v>-2.064738140494073</v>
+        <v>-0.65347581563928314</v>
       </c>
       <c r="D19">
-        <v>1.0523108204895499</v>
+        <v>1.0814564554593771</v>
       </c>
       <c r="E19">
-        <v>-1.9466216198268786</v>
+        <v>-1.1566215140657734</v>
       </c>
       <c r="F19">
-        <v>-1.1873011298234863</v>
+        <v>-0.69796125848796675</v>
       </c>
       <c r="G19">
-        <v>1.4603497100671303</v>
+        <v>1.3453011509757073</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
+        <v>-0.4479223900626072</v>
+      </c>
+      <c r="B20">
+        <v>0.81300981757938984</v>
+      </c>
+      <c r="C20">
         <v>-0.58598066097231494</v>
       </c>
-      <c r="B20">
-        <v>0.95260206927698321</v>
-      </c>
-      <c r="C20">
-        <v>-1.3284273623089653</v>
-      </c>
       <c r="D20">
-        <v>1.5999419617647237</v>
+        <v>1.4588157292792447</v>
       </c>
       <c r="E20">
-        <v>-1.8913983114629955</v>
+        <v>-1.0415729549743504</v>
       </c>
       <c r="F20">
-        <v>-0.86056322200384472</v>
+        <v>-0.80073797127630464</v>
       </c>
       <c r="G20">
-        <v>0.71943698951836565</v>
+        <v>1.1811652066719438</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>-0.27765052260730105</v>
+        <v>-0.25924275315267337</v>
       </c>
       <c r="B21">
-        <v>0.84215545254921698</v>
+        <v>0.65040785406351187</v>
       </c>
       <c r="C21">
-        <v>-1.3176894967937658</v>
+        <v>-0.27458256103152978</v>
       </c>
       <c r="D21">
-        <v>1.8867963690993386</v>
+        <v>1.7088545977046044</v>
       </c>
       <c r="E21">
-        <v>-1.6766410011590058</v>
+        <v>-0.59365056491174317</v>
       </c>
       <c r="F21">
-        <v>-0.9081166264282996</v>
+        <v>-0.84675739491287394</v>
       </c>
       <c r="G21">
-        <v>0.74704864370030721</v>
+        <v>1.227184630308513</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>-3.3747577333484102E-2</v>
+        <v>-0.21322332951610412</v>
       </c>
       <c r="B22">
-        <v>0.6350680461846554</v>
+        <v>0.56910687230557289</v>
       </c>
       <c r="C22">
-        <v>-0.60438843042694257</v>
+        <v>0.5905826033359719</v>
       </c>
       <c r="D22">
-        <v>2.0570682365546449</v>
+        <v>1.7395342134623171</v>
       </c>
       <c r="E22">
-        <v>-0.58751464176020052</v>
+        <v>0.50774764079014723</v>
       </c>
       <c r="F22">
-        <v>-1.2348545342479411</v>
+        <v>-0.69949523927585233</v>
       </c>
       <c r="G22">
-        <v>1.1152040327928612</v>
+        <v>1.4787574795217582</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>0.38963112012295287</v>
+        <v>0.24543692606170259</v>
       </c>
       <c r="B23">
-        <v>0.96027197321641133</v>
+        <v>0.74091272054876467</v>
       </c>
       <c r="C23">
-        <v>0.57064085309345847</v>
+        <v>0.51695152551746104</v>
       </c>
       <c r="D23">
-        <v>1.6229516735830083</v>
+        <v>1.5569904997039259</v>
       </c>
       <c r="E23">
-        <v>1.7686798484321442</v>
+        <v>0.94800012691332625</v>
       </c>
       <c r="F23">
-        <v>-0.80227195206419033</v>
+        <v>-0.73477679739722213</v>
       </c>
       <c r="G23">
-        <v>2.1675148532824111</v>
+        <v>1.727262367159232</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>0.70102922006373802</v>
+        <v>0.5108156023659185</v>
       </c>
       <c r="B24">
-        <v>1.0829904362472627</v>
+        <v>0.88664089539790059</v>
       </c>
       <c r="C24">
-        <v>0.63813600776042678</v>
+        <v>0.5108156023659185</v>
       </c>
       <c r="D24">
-        <v>1.2946797849754812</v>
+        <v>1.1919030721871431</v>
       </c>
       <c r="E24">
-        <v>1.9680973508572777</v>
+        <v>1.047708878125893</v>
       </c>
       <c r="F24">
-        <v>-0.82067972151881807</v>
+        <v>-0.55376706442671642</v>
       </c>
       <c r="G24">
-        <v>2.1920585458885813</v>
+        <v>1.7303303287350031</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>0.66267970036659696</v>
+        <v>0.40497092800180928</v>
       </c>
       <c r="B25">
-        <v>0.92499041509504165</v>
+        <v>0.75849999999999995</v>
       </c>
       <c r="C25">
-        <v>0.69949523927585233</v>
+        <v>0.7040971816395093</v>
       </c>
       <c r="D25">
-        <v>1.2824079386723961</v>
+        <v>1.0952622825503477</v>
       </c>
       <c r="E25">
-        <v>1.9052041385539664</v>
+        <v>1.0293011086712651</v>
       </c>
       <c r="F25">
-        <v>-0.78079622103379132</v>
+        <v>-0.55547579448706197</v>
       </c>
       <c r="G25">
-        <v>1.9466216198268786</v>
+        <v>1.385184651460734</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>0.73477679739722213</v>
+        <v>0.27304858024364415</v>
       </c>
       <c r="B26">
-        <v>0.624330180669456</v>
+        <v>0.72613602891264795</v>
       </c>
       <c r="C26">
-        <v>2.7611654181941541E-2</v>
+        <v>0.65654377721505441</v>
       </c>
       <c r="D26">
-        <v>1.7993594641898571</v>
+        <v>1.4312040750973032</v>
       </c>
       <c r="E26">
-        <v>1.500233210552157</v>
+        <v>1.1305438406717176</v>
       </c>
       <c r="F26">
-        <v>-0.45712627478992107</v>
+        <v>-0.75690000000000002</v>
       </c>
       <c r="G26">
-        <v>2.3270488552225177</v>
+        <v>1.701184693765176</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>0.24236896448593132</v>
+        <v>-8.283496254582462E-2</v>
       </c>
       <c r="B27">
-        <v>0.48473792897186263</v>
+        <v>0.55069910285094514</v>
       </c>
       <c r="C27">
-        <v>0.26384469551633027</v>
+        <v>0.27611654181941542</v>
       </c>
       <c r="D27">
-        <v>2.064738140494073</v>
+        <v>1.6587963479471199</v>
       </c>
       <c r="E27">
-        <v>1.3759807667334201</v>
+        <v>0.31446606151655643</v>
       </c>
       <c r="F27">
-        <v>-0.67341756588179646</v>
+        <v>-0.84675739491287394</v>
       </c>
       <c r="G27">
-        <v>2.2181362192826373</v>
+        <v>1.5293788455219843</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>-1.0139613007924089</v>
+        <v>-0.26231071472844464</v>
       </c>
       <c r="B28">
-        <v>0.61819425751791335</v>
+        <v>0.54302919891151702</v>
       </c>
       <c r="C28">
-        <v>0.12578642460662257</v>
+        <v>-0.32673790781964157</v>
       </c>
       <c r="D28">
-        <v>2.0678061020698442</v>
+        <v>1.6073788666742099</v>
       </c>
       <c r="E28">
-        <v>-0.86056322200384472</v>
+        <v>-0.61972823830579904</v>
       </c>
       <c r="F28">
-        <v>-0.84215545254921698</v>
+        <v>-0.73170883582145085</v>
       </c>
       <c r="G28">
-        <v>0.48933987133551954</v>
+        <v>1.2778059963087391</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>-1.0998642249140047</v>
+        <v>-0.40190296642603801</v>
       </c>
       <c r="B29">
-        <v>0.59211658412385748</v>
+        <v>0.76085447079127799</v>
       </c>
       <c r="C29">
-        <v>-0.33440781175906975</v>
+        <v>-0.59518454569962875</v>
       </c>
       <c r="D29">
-        <v>1.8607186957052828</v>
+        <v>1.4388739790367313</v>
       </c>
       <c r="E29">
-        <v>-1.2716700731571966</v>
+        <v>-0.9648739155800683</v>
       </c>
       <c r="F29">
-        <v>-0.48013598660820567</v>
+        <v>-0.8390874909734457</v>
       </c>
       <c r="G29">
-        <v>0.55990298757825907</v>
+        <v>1.3360972662483934</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>-0.79460204812476209</v>
+        <v>-0.70869912400316626</v>
       </c>
       <c r="B30">
-        <v>0.73324281660933643</v>
+        <v>0.88664089539790059</v>
       </c>
       <c r="C30">
-        <v>-1.0814564554593771</v>
+        <v>-0.63200008460888413</v>
       </c>
       <c r="D30">
-        <v>1.406660382491133</v>
+        <v>1.0858836485505701</v>
       </c>
       <c r="E30">
-        <v>-1.500233210552157</v>
+        <v>-1.201106956914457</v>
       </c>
       <c r="F30">
-        <v>-0.65347581563928314</v>
+        <v>-0.73477679739722213</v>
       </c>
       <c r="G30">
-        <v>1.0415729549743504</v>
+        <v>1.3314953238847365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>